<commit_message>
Tratamiento de datos: considerando estados dependientes o con poco reconocimiento
</commit_message>
<xml_diff>
--- a/data/olympics_excel.xlsx
+++ b/data/olympics_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T172"/>
+  <dimension ref="A1:T171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1695,8 +1695,16 @@
           <t>BER</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>BMU</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>América</t>
+        </is>
+      </c>
       <c r="F18" t="n">
         <v>20</v>
       </c>
@@ -5167,8 +5175,16 @@
           <t>HKG</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>HKG</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
       <c r="F67" t="n">
         <v>18</v>
       </c>
@@ -5735,8 +5751,16 @@
           <t>ISR</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>ISR</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
       <c r="F75" t="n">
         <v>18</v>
       </c>
@@ -8663,8 +8687,16 @@
           <t>PUR</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr"/>
-      <c r="E116" t="inlineStr"/>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>PRI</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>América</t>
+        </is>
+      </c>
       <c r="F116" t="n">
         <v>20</v>
       </c>
@@ -10687,8 +10719,16 @@
           <t>TPE</t>
         </is>
       </c>
-      <c r="D145" t="inlineStr"/>
-      <c r="E145" t="inlineStr"/>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>TWN</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
       <c r="F145" t="n">
         <v>16</v>
       </c>
@@ -10810,46 +10850,46 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Tajikistan (TJK)</t>
+          <t>Tanzania (TAN)</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Tanzania</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TAN</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TZA</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="F147" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I147" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J147" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K147" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L147" t="n">
         <v>0</v>
@@ -10864,64 +10904,64 @@
         <v>0</v>
       </c>
       <c r="P147" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S147" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T147" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Tanzania (TAN)</t>
+          <t>Thailand (THA)</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Tanzania</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>TAN</t>
+          <t>THA</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>TZA</t>
+          <t>THA</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="F148" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G148" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H148" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I148" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J148" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="K148" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L148" t="n">
         <v>0</v>
@@ -10936,64 +10976,64 @@
         <v>0</v>
       </c>
       <c r="P148" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q148" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="R148" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="S148" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="T148" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Thailand (THA)</t>
+          <t>Togo (TOG)</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Togo</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>THA</t>
+          <t>TOG</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>THA</t>
+          <t>TGO</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="F149" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G149" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H149" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I149" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J149" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="K149" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L149" t="n">
         <v>0</v>
@@ -11008,58 +11048,58 @@
         <v>0</v>
       </c>
       <c r="P149" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="Q149" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="R149" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="S149" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="T149" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Togo (TOG)</t>
+          <t>Tonga (TGA)</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Tonga</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>TOG</t>
+          <t>TGA</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>TGO</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceanía</t>
         </is>
       </c>
       <c r="F150" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G150" t="n">
         <v>0</v>
       </c>
       <c r="H150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J150" t="n">
         <v>1</v>
@@ -11080,16 +11120,16 @@
         <v>0</v>
       </c>
       <c r="P150" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q150" t="n">
         <v>0</v>
       </c>
       <c r="R150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T150" t="n">
         <v>1</v>
@@ -11098,46 +11138,46 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Tonga (TGA)</t>
+          <t>Trinidad and Tobago (TTO)</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Tonga</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>TGA</t>
+          <t>TTO</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TTO</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Oceanía</t>
+          <t>América</t>
         </is>
       </c>
       <c r="F151" t="n">
+        <v>19</v>
+      </c>
+      <c r="G151" t="n">
+        <v>3</v>
+      </c>
+      <c r="H151" t="n">
+        <v>5</v>
+      </c>
+      <c r="I151" t="n">
         <v>11</v>
       </c>
-      <c r="G151" t="n">
-        <v>0</v>
-      </c>
-      <c r="H151" t="n">
-        <v>1</v>
-      </c>
-      <c r="I151" t="n">
-        <v>0</v>
-      </c>
       <c r="J151" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="K151" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L151" t="n">
         <v>0</v>
@@ -11152,137 +11192,137 @@
         <v>0</v>
       </c>
       <c r="P151" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="Q151" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R151" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S151" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="T151" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago (TTO)</t>
+          <t>Tunisia (TUN)</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>TTO</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>TTO</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>América</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="F152" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G152" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H152" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I152" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J152" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q152" t="n">
+        <v>6</v>
+      </c>
+      <c r="R152" t="n">
         <v>4</v>
       </c>
-      <c r="L152" t="n">
-        <v>0</v>
-      </c>
-      <c r="M152" t="n">
-        <v>0</v>
-      </c>
-      <c r="N152" t="n">
-        <v>0</v>
-      </c>
-      <c r="O152" t="n">
-        <v>0</v>
-      </c>
-      <c r="P152" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q152" t="n">
-        <v>3</v>
-      </c>
-      <c r="R152" t="n">
-        <v>5</v>
-      </c>
       <c r="S152" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="T152" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Tunisia (TUN)</t>
+          <t>Turkey (TUR)</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>TUR</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>TUR</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Europa</t>
         </is>
       </c>
       <c r="F153" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G153" t="n">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="H153" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="I153" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="J153" t="n">
+        <v>111</v>
+      </c>
+      <c r="K153" t="n">
         <v>18</v>
       </c>
-      <c r="K153" t="n">
-        <v>0</v>
-      </c>
       <c r="L153" t="n">
         <v>0</v>
       </c>
@@ -11296,19 +11336,19 @@
         <v>0</v>
       </c>
       <c r="P153" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="Q153" t="n">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R153" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="S153" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="T153" t="n">
-        <v>18</v>
+        <v>111</v>
       </c>
     </row>
     <row r="154">
@@ -11334,7 +11374,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Europa</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="F154" t="n">
@@ -11386,46 +11426,38 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Turkey (TUR)</t>
+          <t>Turkmenistan (TKM)</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Turkmenistan</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>TUR</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>TUR</t>
-        </is>
-      </c>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>Asia</t>
-        </is>
-      </c>
+          <t>TKM</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
       <c r="F155" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G155" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="H155" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="I155" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J155" t="n">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="K155" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L155" t="n">
         <v>0</v>
@@ -11440,53 +11472,61 @@
         <v>0</v>
       </c>
       <c r="P155" t="n">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="Q155" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="R155" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="S155" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="T155" t="n">
-        <v>111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Turkmenistan (TKM)</t>
+          <t>Uganda (UGA)</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Turkmenistan</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>TKM</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
+          <t>UGA</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>UGA</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
       <c r="F156" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G156" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H156" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I156" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J156" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K156" t="n">
         <v>0</v>
@@ -11504,256 +11544,256 @@
         <v>0</v>
       </c>
       <c r="P156" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Q156" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R156" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S156" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T156" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Uganda (UGA)</t>
+          <t>Ukraine (UKR)</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Europa</t>
         </is>
       </c>
       <c r="F157" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G157" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="H157" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="I157" t="n">
+        <v>72</v>
+      </c>
+      <c r="J157" t="n">
+        <v>151</v>
+      </c>
+      <c r="K157" t="n">
+        <v>8</v>
+      </c>
+      <c r="L157" t="n">
         <v>3</v>
       </c>
-      <c r="J157" t="n">
-        <v>13</v>
-      </c>
-      <c r="K157" t="n">
-        <v>0</v>
-      </c>
-      <c r="L157" t="n">
-        <v>0</v>
-      </c>
       <c r="M157" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N157" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O157" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P157" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q157" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="R157" t="n">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="S157" t="n">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="T157" t="n">
-        <v>13</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Ukraine (UKR)</t>
+          <t>United Arab Emirates (UAE)</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UAE</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>ARE</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Europa</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="F158" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G158" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="H158" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I158" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="J158" t="n">
-        <v>151</v>
+        <v>2</v>
       </c>
       <c r="K158" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L158" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M158" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N158" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O158" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P158" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Q158" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="R158" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="S158" t="n">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="T158" t="n">
-        <v>160</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>United Arab Emirates (UAE)</t>
+          <t>United States (USA)</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>UAE</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>ARE</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>América</t>
         </is>
       </c>
       <c r="F159" t="n">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G159" t="n">
-        <v>1</v>
+        <v>1105</v>
       </c>
       <c r="H159" t="n">
-        <v>0</v>
+        <v>879</v>
       </c>
       <c r="I159" t="n">
-        <v>1</v>
+        <v>780</v>
       </c>
       <c r="J159" t="n">
-        <v>2</v>
+        <v>2764</v>
       </c>
       <c r="K159" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="L159" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="M159" t="n">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="N159" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="O159" t="n">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="P159" t="n">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="Q159" t="n">
-        <v>1</v>
+        <v>1219</v>
       </c>
       <c r="R159" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="S159" t="n">
-        <v>1</v>
+        <v>875</v>
       </c>
       <c r="T159" t="n">
-        <v>2</v>
+        <v>3094</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>United States (USA)</t>
+          <t>Uruguay (URU)</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>URU</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>URY</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -11762,97 +11802,97 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G160" t="n">
-        <v>1105</v>
+        <v>2</v>
       </c>
       <c r="H160" t="n">
-        <v>879</v>
+        <v>2</v>
       </c>
       <c r="I160" t="n">
-        <v>780</v>
+        <v>6</v>
       </c>
       <c r="J160" t="n">
-        <v>2764</v>
+        <v>10</v>
       </c>
       <c r="K160" t="n">
+        <v>1</v>
+      </c>
+      <c r="L160" t="n">
+        <v>0</v>
+      </c>
+      <c r="M160" t="n">
+        <v>0</v>
+      </c>
+      <c r="N160" t="n">
+        <v>0</v>
+      </c>
+      <c r="O160" t="n">
+        <v>0</v>
+      </c>
+      <c r="P160" t="n">
         <v>24</v>
       </c>
-      <c r="L160" t="n">
-        <v>114</v>
-      </c>
-      <c r="M160" t="n">
-        <v>121</v>
-      </c>
-      <c r="N160" t="n">
-        <v>95</v>
-      </c>
-      <c r="O160" t="n">
-        <v>330</v>
-      </c>
-      <c r="P160" t="n">
-        <v>53</v>
-      </c>
       <c r="Q160" t="n">
-        <v>1219</v>
+        <v>2</v>
       </c>
       <c r="R160" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="S160" t="n">
-        <v>875</v>
+        <v>6</v>
       </c>
       <c r="T160" t="n">
-        <v>3094</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Uruguay (URU)</t>
+          <t>Uzbekistan (UZB)</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>URU</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>URY</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>América</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="F161" t="n">
+        <v>8</v>
+      </c>
+      <c r="G161" t="n">
+        <v>18</v>
+      </c>
+      <c r="H161" t="n">
+        <v>8</v>
+      </c>
+      <c r="I161" t="n">
         <v>23</v>
       </c>
-      <c r="G161" t="n">
-        <v>2</v>
-      </c>
-      <c r="H161" t="n">
-        <v>2</v>
-      </c>
-      <c r="I161" t="n">
-        <v>6</v>
-      </c>
       <c r="J161" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="K161" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M161" t="n">
         <v>0</v>
@@ -11861,70 +11901,70 @@
         <v>0</v>
       </c>
       <c r="O161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P161" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="Q161" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="R161" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S161" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="T161" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Uzbekistan (UZB)</t>
+          <t>Venezuela (VEN)</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>VEN</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>VEN</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>América</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G162" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H162" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I162" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="J162" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="K162" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M162" t="n">
         <v>0</v>
@@ -11933,67 +11973,67 @@
         <v>0</v>
       </c>
       <c r="O162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P162" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="Q162" t="n">
+        <v>3</v>
+      </c>
+      <c r="R162" t="n">
+        <v>7</v>
+      </c>
+      <c r="S162" t="n">
+        <v>9</v>
+      </c>
+      <c r="T162" t="n">
         <v>19</v>
-      </c>
-      <c r="R162" t="n">
-        <v>8</v>
-      </c>
-      <c r="S162" t="n">
-        <v>23</v>
-      </c>
-      <c r="T162" t="n">
-        <v>50</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Venezuela (VEN)</t>
+          <t>Vietnam (VIE)</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>VEN</t>
+          <t>VIE</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>VEN</t>
+          <t>VNM</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>América</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G163" t="n">
+        <v>1</v>
+      </c>
+      <c r="H163" t="n">
         <v>3</v>
       </c>
-      <c r="H163" t="n">
-        <v>7</v>
-      </c>
       <c r="I163" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J163" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="K163" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L163" t="n">
         <v>0</v>
@@ -12008,64 +12048,56 @@
         <v>0</v>
       </c>
       <c r="P163" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="Q163" t="n">
+        <v>1</v>
+      </c>
+      <c r="R163" t="n">
         <v>3</v>
       </c>
-      <c r="R163" t="n">
-        <v>7</v>
-      </c>
       <c r="S163" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="T163" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Vietnam (VIE)</t>
+          <t>Virgin Islands (ISV)</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Virgin Islands</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>VIE</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>VNM</t>
-        </is>
-      </c>
-      <c r="E164" t="inlineStr">
-        <is>
-          <t>Asia</t>
-        </is>
-      </c>
+          <t>ISV</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr"/>
       <c r="F164" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H164" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J164" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K164" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L164" t="n">
         <v>0</v>
@@ -12080,168 +12112,176 @@
         <v>0</v>
       </c>
       <c r="P164" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Q164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R164" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T164" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Virgin Islands (ISV)</t>
+          <t>Yugoslavia (YUG)</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Virgin Islands</t>
+          <t>Yugoslavia</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>ISV</t>
+          <t>YUG</t>
         </is>
       </c>
       <c r="D165" t="inlineStr"/>
       <c r="E165" t="inlineStr"/>
       <c r="F165" t="n">
+        <v>16</v>
+      </c>
+      <c r="G165" t="n">
+        <v>26</v>
+      </c>
+      <c r="H165" t="n">
+        <v>29</v>
+      </c>
+      <c r="I165" t="n">
+        <v>28</v>
+      </c>
+      <c r="J165" t="n">
+        <v>83</v>
+      </c>
+      <c r="K165" t="n">
         <v>14</v>
       </c>
-      <c r="G165" t="n">
-        <v>0</v>
-      </c>
-      <c r="H165" t="n">
-        <v>1</v>
-      </c>
-      <c r="I165" t="n">
-        <v>0</v>
-      </c>
-      <c r="J165" t="n">
-        <v>1</v>
-      </c>
-      <c r="K165" t="n">
-        <v>8</v>
-      </c>
       <c r="L165" t="n">
         <v>0</v>
       </c>
       <c r="M165" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O165" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P165" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="Q165" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="R165" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="S165" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="T165" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Yugoslavia (YUG)</t>
+          <t>Zambia (ZAM)</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Yugoslavia</t>
+          <t>Zambia</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>YUG</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr"/>
+          <t>ZAM</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>ZMB</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
       <c r="F166" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G166" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="H166" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="I166" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J166" t="n">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="K166" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L166" t="n">
         <v>0</v>
       </c>
       <c r="M166" t="n">
+        <v>0</v>
+      </c>
+      <c r="N166" t="n">
+        <v>0</v>
+      </c>
+      <c r="O166" t="n">
+        <v>0</v>
+      </c>
+      <c r="P166" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q166" t="n">
+        <v>0</v>
+      </c>
+      <c r="R166" t="n">
+        <v>1</v>
+      </c>
+      <c r="S166" t="n">
+        <v>2</v>
+      </c>
+      <c r="T166" t="n">
         <v>3</v>
-      </c>
-      <c r="N166" t="n">
-        <v>1</v>
-      </c>
-      <c r="O166" t="n">
-        <v>4</v>
-      </c>
-      <c r="P166" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q166" t="n">
-        <v>26</v>
-      </c>
-      <c r="R166" t="n">
-        <v>32</v>
-      </c>
-      <c r="S166" t="n">
-        <v>29</v>
-      </c>
-      <c r="T166" t="n">
-        <v>87</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Zambia (ZAM)</t>
+          <t>Zimbabwe (ZIM)</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Zambia</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>ZAM</t>
+          <t>ZIM</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>ZMB</t>
+          <t>ZWE</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -12253,91 +12293,83 @@
         <v>15</v>
       </c>
       <c r="G167" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H167" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J167" t="n">
+        <v>8</v>
+      </c>
+      <c r="K167" t="n">
+        <v>1</v>
+      </c>
+      <c r="L167" t="n">
+        <v>0</v>
+      </c>
+      <c r="M167" t="n">
+        <v>0</v>
+      </c>
+      <c r="N167" t="n">
+        <v>0</v>
+      </c>
+      <c r="O167" t="n">
+        <v>0</v>
+      </c>
+      <c r="P167" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q167" t="n">
         <v>3</v>
       </c>
-      <c r="K167" t="n">
-        <v>0</v>
-      </c>
-      <c r="L167" t="n">
-        <v>0</v>
-      </c>
-      <c r="M167" t="n">
-        <v>0</v>
-      </c>
-      <c r="N167" t="n">
-        <v>0</v>
-      </c>
-      <c r="O167" t="n">
-        <v>0</v>
-      </c>
-      <c r="P167" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q167" t="n">
-        <v>0</v>
-      </c>
       <c r="R167" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T167" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Zimbabwe (ZIM)</t>
+          <t>Individual Neutral Athletes (AIN)</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>Individual Neutral Athletes</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>ZIM</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>ZWE</t>
-        </is>
-      </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>Africa</t>
-        </is>
-      </c>
+          <t>AIN</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr"/>
       <c r="F168" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G168" t="n">
+        <v>1</v>
+      </c>
+      <c r="H168" t="n">
         <v>3</v>
       </c>
-      <c r="H168" t="n">
-        <v>4</v>
-      </c>
       <c r="I168" t="n">
         <v>1</v>
       </c>
       <c r="J168" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K168" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L168" t="n">
         <v>0</v>
@@ -12352,118 +12384,118 @@
         <v>0</v>
       </c>
       <c r="P168" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="Q168" t="n">
+        <v>1</v>
+      </c>
+      <c r="R168" t="n">
         <v>3</v>
       </c>
-      <c r="R168" t="n">
-        <v>4</v>
-      </c>
       <c r="S168" t="n">
         <v>1</v>
       </c>
       <c r="T168" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Individual Neutral Athletes (AIN)</t>
+          <t>Independent Olympic Athletes (IOA)</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Individual Neutral Athletes</t>
+          <t>Independent Olympic Athletes</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>AIN</t>
+          <t>IOA</t>
         </is>
       </c>
       <c r="D169" t="inlineStr"/>
       <c r="E169" t="inlineStr"/>
       <c r="F169" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G169" t="n">
         <v>1</v>
       </c>
       <c r="H169" t="n">
+        <v>0</v>
+      </c>
+      <c r="I169" t="n">
+        <v>1</v>
+      </c>
+      <c r="J169" t="n">
+        <v>2</v>
+      </c>
+      <c r="K169" t="n">
+        <v>0</v>
+      </c>
+      <c r="L169" t="n">
+        <v>0</v>
+      </c>
+      <c r="M169" t="n">
+        <v>0</v>
+      </c>
+      <c r="N169" t="n">
+        <v>0</v>
+      </c>
+      <c r="O169" t="n">
+        <v>0</v>
+      </c>
+      <c r="P169" t="n">
         <v>3</v>
       </c>
-      <c r="I169" t="n">
-        <v>1</v>
-      </c>
-      <c r="J169" t="n">
-        <v>5</v>
-      </c>
-      <c r="K169" t="n">
-        <v>0</v>
-      </c>
-      <c r="L169" t="n">
-        <v>0</v>
-      </c>
-      <c r="M169" t="n">
-        <v>0</v>
-      </c>
-      <c r="N169" t="n">
-        <v>0</v>
-      </c>
-      <c r="O169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P169" t="n">
-        <v>1</v>
-      </c>
       <c r="Q169" t="n">
         <v>1</v>
       </c>
       <c r="R169" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S169" t="n">
         <v>1</v>
       </c>
       <c r="T169" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Independent Olympic Athletes (IOA)</t>
+          <t>Independent Olympic Participants (IOP)</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Independent Olympic Athletes</t>
+          <t>Independent Olympic Participants</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>IOA</t>
+          <t>IOP</t>
         </is>
       </c>
       <c r="D170" t="inlineStr"/>
       <c r="E170" t="inlineStr"/>
       <c r="F170" t="n">
+        <v>1</v>
+      </c>
+      <c r="G170" t="n">
+        <v>0</v>
+      </c>
+      <c r="H170" t="n">
+        <v>1</v>
+      </c>
+      <c r="I170" t="n">
+        <v>2</v>
+      </c>
+      <c r="J170" t="n">
         <v>3</v>
       </c>
-      <c r="G170" t="n">
-        <v>1</v>
-      </c>
-      <c r="H170" t="n">
-        <v>0</v>
-      </c>
-      <c r="I170" t="n">
-        <v>1</v>
-      </c>
-      <c r="J170" t="n">
-        <v>2</v>
-      </c>
       <c r="K170" t="n">
         <v>0</v>
       </c>
@@ -12480,146 +12512,82 @@
         <v>0</v>
       </c>
       <c r="P170" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q170" t="n">
+        <v>0</v>
+      </c>
+      <c r="R170" t="n">
+        <v>1</v>
+      </c>
+      <c r="S170" t="n">
+        <v>2</v>
+      </c>
+      <c r="T170" t="n">
         <v>3</v>
-      </c>
-      <c r="Q170" t="n">
-        <v>1</v>
-      </c>
-      <c r="R170" t="n">
-        <v>0</v>
-      </c>
-      <c r="S170" t="n">
-        <v>1</v>
-      </c>
-      <c r="T170" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Independent Olympic Participants (IOP)</t>
+          <t>Mixed team (ZZX)</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Independent Olympic Participants</t>
+          <t>Mixed team</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>IOP</t>
+          <t>ZZX</t>
         </is>
       </c>
       <c r="D171" t="inlineStr"/>
       <c r="E171" t="inlineStr"/>
       <c r="F171" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G171" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H171" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I171" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J171" t="n">
+        <v>25</v>
+      </c>
+      <c r="K171" t="n">
+        <v>0</v>
+      </c>
+      <c r="L171" t="n">
+        <v>0</v>
+      </c>
+      <c r="M171" t="n">
+        <v>0</v>
+      </c>
+      <c r="N171" t="n">
+        <v>0</v>
+      </c>
+      <c r="O171" t="n">
+        <v>0</v>
+      </c>
+      <c r="P171" t="n">
         <v>3</v>
       </c>
-      <c r="K171" t="n">
-        <v>0</v>
-      </c>
-      <c r="L171" t="n">
-        <v>0</v>
-      </c>
-      <c r="M171" t="n">
-        <v>0</v>
-      </c>
-      <c r="N171" t="n">
-        <v>0</v>
-      </c>
-      <c r="O171" t="n">
-        <v>0</v>
-      </c>
-      <c r="P171" t="n">
-        <v>1</v>
-      </c>
       <c r="Q171" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="R171" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S171" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="T171" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>Mixed team (ZZX)</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>Mixed team</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>ZZX</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr"/>
-      <c r="E172" t="inlineStr"/>
-      <c r="F172" t="n">
-        <v>3</v>
-      </c>
-      <c r="G172" t="n">
-        <v>11</v>
-      </c>
-      <c r="H172" t="n">
-        <v>6</v>
-      </c>
-      <c r="I172" t="n">
-        <v>8</v>
-      </c>
-      <c r="J172" t="n">
-        <v>25</v>
-      </c>
-      <c r="K172" t="n">
-        <v>0</v>
-      </c>
-      <c r="L172" t="n">
-        <v>0</v>
-      </c>
-      <c r="M172" t="n">
-        <v>0</v>
-      </c>
-      <c r="N172" t="n">
-        <v>0</v>
-      </c>
-      <c r="O172" t="n">
-        <v>0</v>
-      </c>
-      <c r="P172" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q172" t="n">
-        <v>11</v>
-      </c>
-      <c r="R172" t="n">
-        <v>6</v>
-      </c>
-      <c r="S172" t="n">
-        <v>8</v>
-      </c>
-      <c r="T172" t="n">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección de errores en el tratamiento de datos, y adición de Indicadores del Banco Mundial para analisis de correlación
</commit_message>
<xml_diff>
--- a/data/olympics_excel.xlsx
+++ b/data/olympics_excel.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ISO_3166-1</t>
+          <t>ISO_code</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -5923,7 +5923,11 @@
           <t>KOS</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>XKX</t>
+        </is>
+      </c>
       <c r="E77" t="inlineStr">
         <is>
           <t>Europa</t>
@@ -11571,7 +11575,11 @@
           <t>ISV</t>
         </is>
       </c>
-      <c r="D156" t="inlineStr"/>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>VIR</t>
+        </is>
+      </c>
       <c r="E156" t="inlineStr">
         <is>
           <t>América</t>

</xml_diff>